<commit_message>
Updated 2/16/22. MFD Level 5 > 4. CAK Level 7 > 4.
</commit_message>
<xml_diff>
--- a/1. Personal Information.xlsx
+++ b/1. Personal Information.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\ERRPDFFill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D8C5EF-26B1-40B4-A036-9D35C610CC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C09E05-E126-4AD7-8A9B-A6609BC182F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Personal Information" sheetId="2" r:id="rId1"/>
@@ -6433,7 +6433,7 @@
       </c>
       <c r="J11" s="16">
         <f ca="1">TODAY()</f>
-        <v>44584</v>
+        <v>44608</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -7052,7 +7052,7 @@
   <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7565,8 +7565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAEA2A4-C887-4AB7-96BA-4474404171DC}">
   <dimension ref="A1:P315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10197,7 +10197,7 @@
         <v>39</v>
       </c>
       <c r="D52" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>1027</v>
@@ -10227,7 +10227,7 @@
       </c>
       <c r="N52" t="str" cm="1">
         <f t="array" ref="N52">_xlfn.IFS(D52=4,"D",D52=5,"E",D52=6,"F",D52=7,"G",D52=8,"H", D52=9, "I", D52=10, "J", D52=11, "K", D52=12, "L")</f>
-        <v>G</v>
+        <v>D</v>
       </c>
       <c r="O52" t="str" cm="1">
         <f t="array" ref="O52">_xlfn.IFS(Table13[[#This Row],[FacilityType]]="Approach control", "2", Table13[[#This Row],[FacilityType]]="Tower and Approach Control", "3", Table13[[#This Row],[FacilityType]]="Combined Control Facility", "6", Table13[[#This Row],[FacilityType]]="Tower", "7", Table13[[#This Row],[FacilityType]]="Enroute Center", "8")</f>
@@ -16337,7 +16337,7 @@
         <v>39</v>
       </c>
       <c r="D170" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>1001</v>
@@ -16367,7 +16367,7 @@
       </c>
       <c r="N170" t="str" cm="1">
         <f t="array" ref="N170">_xlfn.IFS(D170=4,"D",D170=5,"E",D170=6,"F",D170=7,"G",D170=8,"H", D170=9, "I", D170=10, "J", D170=11, "K", D170=12, "L")</f>
-        <v>E</v>
+        <v>D</v>
       </c>
       <c r="O170" t="str" cm="1">
         <f t="array" ref="O170">_xlfn.IFS(Table13[[#This Row],[FacilityType]]="Approach control", "2", Table13[[#This Row],[FacilityType]]="Tower and Approach Control", "3", Table13[[#This Row],[FacilityType]]="Combined Control Facility", "6", Table13[[#This Row],[FacilityType]]="Tower", "7", Table13[[#This Row],[FacilityType]]="Enroute Center", "8")</f>
@@ -23779,6 +23779,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
@@ -23792,7 +23793,7 @@
   <dimension ref="A1:P315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:P1048576"/>
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26423,7 +26424,7 @@
         <v>39</v>
       </c>
       <c r="D52" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>1027</v>
@@ -26453,7 +26454,7 @@
       </c>
       <c r="N52" t="str" cm="1">
         <f t="array" ref="N52">_xlfn.IFS(D52=4,"D",D52=5,"E",D52=6,"F",D52=7,"G",D52=8,"H", D52=9, "I", D52=10, "J", D52=11, "K", D52=12, "L")</f>
-        <v>G</v>
+        <v>D</v>
       </c>
       <c r="O52" t="str" cm="1">
         <f t="array" ref="O52">_xlfn.IFS(Table1[[#This Row],[FacilityType]]="Approach control", "2", Table1[[#This Row],[FacilityType]]="Tower and Approach Control", "3", Table1[[#This Row],[FacilityType]]="Combined Control Facility", "6", Table1[[#This Row],[FacilityType]]="Tower", "7", Table1[[#This Row],[FacilityType]]="Enroute Center", "8")</f>
@@ -32563,7 +32564,7 @@
         <v>39</v>
       </c>
       <c r="D170" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>1001</v>
@@ -32593,7 +32594,7 @@
       </c>
       <c r="N170" t="str" cm="1">
         <f t="array" ref="N170">_xlfn.IFS(D170=4,"D",D170=5,"E",D170=6,"F",D170=7,"G",D170=8,"H", D170=9, "I", D170=10, "J", D170=11, "K", D170=12, "L")</f>
-        <v>E</v>
+        <v>D</v>
       </c>
       <c r="O170" t="str" cm="1">
         <f t="array" ref="O170">_xlfn.IFS(Table1[[#This Row],[FacilityType]]="Approach control", "2", Table1[[#This Row],[FacilityType]]="Tower and Approach Control", "3", Table1[[#This Row],[FacilityType]]="Combined Control Facility", "6", Table1[[#This Row],[FacilityType]]="Tower", "7", Table1[[#This Row],[FacilityType]]="Enroute Center", "8")</f>
@@ -40170,7 +40171,7 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>23 January 2022</v>
+        <v>16 February 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -40179,7 +40180,7 @@
       </c>
       <c r="B17" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>01/23/22</v>
+        <v>02/16/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -41657,7 +41658,7 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>23 January 2022</v>
+        <v>16 February 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -41666,7 +41667,7 @@
       </c>
       <c r="B17" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>01/23/22</v>
+        <v>02/16/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -43143,7 +43144,7 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>23 January 2022</v>
+        <v>16 February 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -43152,7 +43153,7 @@
       </c>
       <c r="B17" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>01/23/22</v>
+        <v>02/16/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -44629,7 +44630,7 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>23 January 2022</v>
+        <v>16 February 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -44638,7 +44639,7 @@
       </c>
       <c r="B17" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>01/23/22</v>
+        <v>02/16/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -46115,7 +46116,7 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>23 January 2022</v>
+        <v>16 February 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -46124,7 +46125,7 @@
       </c>
       <c r="B17" t="str">
         <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>01/23/22</v>
+        <v>02/16/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated 3/12/22. Added function to automatically attach resume & performance plan pdfs to each generated package. Moved all generated packages to single folder. Removed extra instructions pages from 3330-43-1. General code reformatting/readability improvements.
</commit_message>
<xml_diff>
--- a/1. Personal Information.xlsx
+++ b/1. Personal Information.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\ERRPDFFill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C09E05-E126-4AD7-8A9B-A6609BC182F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E73E809-B5A0-4D48-AF17-0B65767F0250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="2115" windowWidth="29070" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Personal Information" sheetId="2" r:id="rId1"/>
@@ -3713,9 +3713,6 @@
     <t>OVERRIDE</t>
   </si>
   <si>
-    <t>Today's date will be used for the date on each form. To override with a different date, type a date in the "OVERRIDE" field. Otherwise, leave "OVERRIDE" blank.</t>
-  </si>
-  <si>
     <t>TodaysDate</t>
   </si>
   <si>
@@ -3962,6 +3959,9 @@
   </si>
   <si>
     <t>Once you complete this sheet, you may save the document and proceed to Step 2.</t>
+  </si>
+  <si>
+    <t>Today's date will be used for the date on each form. To override with a different date, type a date in the "OVERRIDE" field. You may also force date fields to be blank by inserting a space in the "OVERRIDE" field. Otherwise, leave "OVERRIDE" blank.</t>
   </si>
 </sst>
 </file>
@@ -4318,7 +4318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -4514,6 +4514,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4560,7 +4578,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4645,14 +4663,20 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="20" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="12" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="20" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="20" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="20" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -6323,7 +6347,7 @@
   <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6340,7 +6364,7 @@
   <sheetData>
     <row r="2" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -6350,7 +6374,7 @@
     </row>
     <row r="4" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -6359,25 +6383,25 @@
       <c r="G4" s="29"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>712</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="34" t="s">
         <v>727</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="4"/>
       <c r="I6" s="33" t="s">
         <v>1213</v>
       </c>
       <c r="J6" s="33"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C7" s="18"/>
       <c r="F7" s="10" t="s">
@@ -6386,75 +6410,77 @@
       <c r="G7" s="10" t="s">
         <v>725</v>
       </c>
-      <c r="I7" s="34" t="s">
-        <v>1215</v>
-      </c>
-      <c r="J7" s="34"/>
+      <c r="I7" s="36" t="s">
+        <v>1277</v>
+      </c>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C8" s="20"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C9" s="21"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="I11" s="5" t="s">
-        <v>1213</v>
-      </c>
-      <c r="J11" s="16">
-        <f ca="1">TODAY()</f>
-        <v>44608</v>
-      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C12" s="22"/>
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
       <c r="I12" s="5" t="s">
-        <v>1214</v>
-      </c>
-      <c r="J12" s="19"/>
+        <v>1213</v>
+      </c>
+      <c r="J12" s="16">
+        <f ca="1">TODAY()</f>
+        <v>44632</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="19"/>
+      <c r="I13" s="5" t="s">
+        <v>1214</v>
+      </c>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
@@ -6503,7 +6529,7 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="4"/>
@@ -6513,7 +6539,7 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C21" s="20"/>
     </row>
@@ -6529,7 +6555,7 @@
       </c>
       <c r="C23" s="31"/>
       <c r="F23" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="G23" s="18"/>
     </row>
@@ -6596,17 +6622,17 @@
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="9">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J10"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="I7:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -6782,16 +6808,16 @@
         <v>0</v>
       </c>
       <c r="L1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="M1" t="s">
         <v>1223</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>1224</v>
       </c>
-      <c r="N1" t="s">
-        <v>1225</v>
-      </c>
       <c r="O1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -6812,13 +6838,13 @@
         <v>33</v>
       </c>
       <c r="M2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="N2" t="s">
         <v>1226</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>1227</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6833,13 +6859,13 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="N3" t="s">
         <v>1229</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>1230</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1231</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -6857,16 +6883,16 @@
         <v>729</v>
       </c>
       <c r="L4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="M4" t="s">
         <v>1233</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>1234</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>1235</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1236</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6884,16 +6910,16 @@
         <v>730</v>
       </c>
       <c r="L5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="M5" t="s">
         <v>1237</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>1238</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>1239</v>
-      </c>
-      <c r="O5" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -6904,16 +6930,16 @@
         <v>731</v>
       </c>
       <c r="L6" t="s">
+        <v>1240</v>
+      </c>
+      <c r="M6" t="s">
         <v>1241</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>1242</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>1243</v>
-      </c>
-      <c r="O6" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -6931,16 +6957,16 @@
         <v>732</v>
       </c>
       <c r="L7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="M7" t="s">
         <v>1245</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>1246</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>1247</v>
-      </c>
-      <c r="O7" t="s">
-        <v>1248</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -6952,22 +6978,22 @@
         <v>#N/A</v>
       </c>
       <c r="G8" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="H8" t="s">
         <v>733</v>
       </c>
       <c r="L8" t="s">
+        <v>1248</v>
+      </c>
+      <c r="M8" t="s">
         <v>1249</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>1250</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>1251</v>
-      </c>
-      <c r="O8" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -6979,22 +7005,22 @@
         <v>#N/A</v>
       </c>
       <c r="G9" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="H9" t="s">
         <v>734</v>
       </c>
       <c r="L9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="M9" t="s">
         <v>1253</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>1254</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>1255</v>
-      </c>
-      <c r="O9" t="s">
-        <v>1256</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -7006,7 +7032,7 @@
         <v>#N/A</v>
       </c>
       <c r="G10" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H10" t="s">
         <v>735</v>
@@ -7052,7 +7078,7 @@
   <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7066,7 +7092,7 @@
   <sheetData>
     <row r="2" spans="2:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -7084,7 +7110,7 @@
     </row>
     <row r="4" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -7094,7 +7120,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
@@ -7255,7 +7281,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B2:G2"/>
@@ -7566,7 +7592,7 @@
   <dimension ref="A1:P315"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7660,7 +7686,7 @@
         <v>763</v>
       </c>
       <c r="G3" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -8543,7 +8569,7 @@
         <v>763</v>
       </c>
       <c r="G20" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
@@ -12494,7 +12520,7 @@
         <v>763</v>
       </c>
       <c r="G96" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H96" t="s">
         <v>14</v>
@@ -15044,7 +15070,7 @@
         <v>763</v>
       </c>
       <c r="G145" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H145" t="s">
         <v>14</v>
@@ -16970,7 +16996,7 @@
         <v>763</v>
       </c>
       <c r="G182" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H182" t="s">
         <v>14</v>
@@ -22787,7 +22813,7 @@
         <v>763</v>
       </c>
       <c r="G294" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="I294" t="s">
         <v>15</v>
@@ -23887,7 +23913,7 @@
         <v>763</v>
       </c>
       <c r="G3" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -24770,7 +24796,7 @@
         <v>763</v>
       </c>
       <c r="G20" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
@@ -28721,7 +28747,7 @@
         <v>763</v>
       </c>
       <c r="G96" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H96" t="s">
         <v>14</v>
@@ -31271,7 +31297,7 @@
         <v>763</v>
       </c>
       <c r="G145" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H145" t="s">
         <v>14</v>
@@ -33197,7 +33223,7 @@
         <v>763</v>
       </c>
       <c r="G182" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H182" t="s">
         <v>14</v>
@@ -39014,7 +39040,7 @@
         <v>763</v>
       </c>
       <c r="G294" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="I294" t="s">
         <v>15</v>
@@ -40086,7 +40112,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B7" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!M1:M9)</f>
@@ -40095,7 +40121,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B8" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!N1:N9)</f>
@@ -40104,7 +40130,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B9" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!O1:O9)</f>
@@ -40167,11 +40193,11 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B16" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>16 February 2022</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"), TEXT('1. Personal Information'!J13, "dd mmmm yyyy"))</f>
+        <v>12 March 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -40179,13 +40205,13 @@
         <v>1213</v>
       </c>
       <c r="B17" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>02/16/22</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "mm/dd/yy"), TEXT('1. Personal Information'!J13, "mm/dd/yy"))</f>
+        <v>03/12/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" t="e">
         <f>_xlfn.CONCAT("FAA ", B5, " Regional Office")</f>
@@ -40194,15 +40220,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B19" t="s">
         <v>1218</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B20" t="e">
         <f>_xlfn.CONCAT("ATTN: ", B7)</f>
@@ -40211,7 +40237,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" t="e">
         <f>B8</f>
@@ -40220,7 +40246,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" t="e">
         <f>B9</f>
@@ -40229,7 +40255,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" t="e">
         <f>_xlfn.CONCAT(B2," (",B1,").")</f>
@@ -41573,7 +41599,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B7" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!M1:M9)</f>
@@ -41582,7 +41608,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B8" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!N1:N9)</f>
@@ -41591,7 +41617,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B9" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!O1:O9)</f>
@@ -41654,11 +41680,11 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B16" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>16 February 2022</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"), TEXT('1. Personal Information'!J13, "dd mmmm yyyy"))</f>
+        <v>12 March 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -41666,13 +41692,13 @@
         <v>1213</v>
       </c>
       <c r="B17" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>02/16/22</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "mm/dd/yy"), TEXT('1. Personal Information'!J13, "mm/dd/yy"))</f>
+        <v>03/12/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" t="e">
         <f>_xlfn.CONCAT("FAA ", B5, " Regional Office")</f>
@@ -41681,15 +41707,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B19" t="s">
         <v>1218</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B20" t="e">
         <f>_xlfn.CONCAT("ATTN: ", B7)</f>
@@ -41698,7 +41724,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" t="e">
         <f>B8</f>
@@ -41707,7 +41733,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" t="e">
         <f>B9</f>
@@ -41716,7 +41742,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" t="e">
         <f>_xlfn.CONCAT(B2," (",B1,").")</f>
@@ -43059,7 +43085,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B7" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!M1:M9)</f>
@@ -43068,7 +43094,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B8" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!N1:N9)</f>
@@ -43077,7 +43103,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B9" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!O1:O9)</f>
@@ -43140,11 +43166,11 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B16" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>16 February 2022</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"), TEXT('1. Personal Information'!J13, "dd mmmm yyyy"))</f>
+        <v>12 March 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -43152,13 +43178,13 @@
         <v>1213</v>
       </c>
       <c r="B17" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>02/16/22</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "mm/dd/yy"), TEXT('1. Personal Information'!J13, "mm/dd/yy"))</f>
+        <v>03/12/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" t="e">
         <f>_xlfn.CONCAT("FAA ", B5, " Regional Office")</f>
@@ -43167,15 +43193,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B19" t="s">
         <v>1218</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B20" t="e">
         <f>_xlfn.CONCAT("ATTN: ", B7)</f>
@@ -43184,7 +43210,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" t="e">
         <f>B8</f>
@@ -43193,7 +43219,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" t="e">
         <f>B9</f>
@@ -43202,7 +43228,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" t="e">
         <f>_xlfn.CONCAT(B2," (",B1,").")</f>
@@ -44545,7 +44571,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B7" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!M1:M9)</f>
@@ -44554,7 +44580,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B8" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!N1:N9)</f>
@@ -44563,7 +44589,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B9" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!O1:O9)</f>
@@ -44626,11 +44652,11 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B16" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>16 February 2022</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"), TEXT('1. Personal Information'!J13, "dd mmmm yyyy"))</f>
+        <v>12 March 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -44638,13 +44664,13 @@
         <v>1213</v>
       </c>
       <c r="B17" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>02/16/22</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "mm/dd/yy"), TEXT('1. Personal Information'!J13, "mm/dd/yy"))</f>
+        <v>03/12/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" t="e">
         <f>_xlfn.CONCAT("FAA ", B5, " Regional Office")</f>
@@ -44653,15 +44679,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B19" t="s">
         <v>1218</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B20" t="e">
         <f>_xlfn.CONCAT("ATTN: ", B7)</f>
@@ -44670,7 +44696,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" t="e">
         <f>B8</f>
@@ -44679,7 +44705,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" t="e">
         <f>B9</f>
@@ -44688,7 +44714,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" t="e">
         <f>_xlfn.CONCAT(B2," (",B1,").")</f>
@@ -46031,7 +46057,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B7" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!M1:M9)</f>
@@ -46040,7 +46066,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B8" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!N1:N9)</f>
@@ -46049,7 +46075,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B9" t="e">
         <f>LOOKUP(B5,Backend!L1:L9,Backend!O1:O9)</f>
@@ -46112,11 +46138,11 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B16" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "dd mmmm yyyy"), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"))</f>
-        <v>16 February 2022</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "dd mmmm yyyy"), TEXT('1. Personal Information'!J13, "dd mmmm yyyy"))</f>
+        <v>12 March 2022</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -46124,13 +46150,13 @@
         <v>1213</v>
       </c>
       <c r="B17" t="str">
-        <f ca="1">IF(ISBLANK('1. Personal Information'!J12), TEXT('1. Personal Information'!J11, "mm/dd/yy"), TEXT('1. Personal Information'!J12, "mm/dd/yy"))</f>
-        <v>02/16/22</v>
+        <f ca="1">IF(ISBLANK('1. Personal Information'!J13), TEXT('1. Personal Information'!J12, "mm/dd/yy"), TEXT('1. Personal Information'!J13, "mm/dd/yy"))</f>
+        <v>03/12/22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" t="e">
         <f>_xlfn.CONCAT("FAA ", B5, " Regional Office")</f>
@@ -46139,15 +46165,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B19" t="s">
         <v>1218</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B20" t="e">
         <f>_xlfn.CONCAT("ATTN: ", B7)</f>
@@ -46156,7 +46182,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" t="e">
         <f>B8</f>
@@ -46165,7 +46191,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" t="e">
         <f>B9</f>
@@ -46174,7 +46200,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" t="e">
         <f>_xlfn.CONCAT(B2," (",B1,").")</f>

</xml_diff>

<commit_message>
Updated 3/12/22. Rev 2: Fixed bug where lowercase facility IDs in excel document would not properly capitalize when generating packages.
</commit_message>
<xml_diff>
--- a/1. Personal Information.xlsx
+++ b/1. Personal Information.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\ERRPDFFill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E73E809-B5A0-4D48-AF17-0B65767F0250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2981A7-5B46-4E28-86B6-FA93CB040C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="2115" windowWidth="29070" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="2460" windowWidth="29070" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Personal Information" sheetId="2" r:id="rId1"/>
@@ -6347,7 +6347,7 @@
   <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G24" sqref="G23:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40047,7 +40047,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40061,7 +40061,7 @@
         <v>807</v>
       </c>
       <c r="B1" t="str">
-        <f>IF(NOT(ISBLANK('1. Personal Information'!G23)), '1. Personal Information'!G23, "")</f>
+        <f>IF(NOT(ISBLANK('1. Personal Information'!G23)), UPPER('1. Personal Information'!G23), "")</f>
         <v/>
       </c>
     </row>
@@ -41534,7 +41534,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41548,7 +41548,7 @@
         <v>807</v>
       </c>
       <c r="B1" t="str">
-        <f>IF(NOT(ISBLANK('1. Personal Information'!G24)), '1. Personal Information'!G24, "")</f>
+        <f>IF(NOT(ISBLANK('1. Personal Information'!G24)), UPPER('1. Personal Information'!G24), "")</f>
         <v/>
       </c>
     </row>
@@ -43020,7 +43020,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43034,7 +43034,7 @@
         <v>807</v>
       </c>
       <c r="B1" t="str">
-        <f>IF(NOT(ISBLANK('1. Personal Information'!G25)), '1. Personal Information'!G25, "")</f>
+        <f>IF(NOT(ISBLANK('1. Personal Information'!G25)), UPPER('1. Personal Information'!G25), "")</f>
         <v/>
       </c>
     </row>
@@ -44506,7 +44506,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44520,7 +44520,7 @@
         <v>807</v>
       </c>
       <c r="B1" t="str">
-        <f>IF(NOT(ISBLANK('1. Personal Information'!G26)), '1. Personal Information'!G26, "")</f>
+        <f>IF(NOT(ISBLANK('1. Personal Information'!G26)), UPPER('1. Personal Information'!G26), "")</f>
         <v/>
       </c>
     </row>
@@ -45992,7 +45992,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46006,7 +46006,7 @@
         <v>807</v>
       </c>
       <c r="B1" t="str">
-        <f>IF(NOT(ISBLANK('1. Personal Information'!G27)), '1. Personal Information'!G27, "")</f>
+        <f>IF(NOT(ISBLANK('1. Personal Information'!G27)), UPPER('1. Personal Information'!G27), "")</f>
         <v/>
       </c>
     </row>

</xml_diff>